<commit_message>
Updated dataset uncertainty (correction to the scaling), implemented more script functionality
</commit_message>
<xml_diff>
--- a/Circuit/circuit_diode_data.xlsx
+++ b/Circuit/circuit_diode_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruich\Documents\GitHub\PHY224-2025\Circuit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruich\Documents\GitHub\School\PHY224-2025\Circuit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452D78DC-30DE-4A9D-9387-C04B602CE8EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4C9E67-4789-4BE0-A94A-24E1353A0D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DCDB4AC7-95AF-412F-A7D4-AE4A32B44ACE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DCDB4AC7-95AF-412F-A7D4-AE4A32B44ACE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -431,25 +431,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1724A488-CA27-4EF9-97DA-F8A5C8AF219E}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.90625" customWidth="1"/>
-    <col min="2" max="2" width="21.54296875" customWidth="1"/>
-    <col min="3" max="3" width="25.26953125" customWidth="1"/>
-    <col min="4" max="4" width="14.90625" customWidth="1"/>
-    <col min="5" max="5" width="18.7265625" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -466,7 +466,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-1.4</v>
       </c>
@@ -482,11 +482,11 @@
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="E3">
-        <f>0.0002*ABS(C3)+0.00000005</f>
-        <v>5.1999999999999996E-8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <f>0.0002*ABS(C3)+0.00005</f>
+        <v>5.0002E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-1.3</v>
       </c>
@@ -502,11 +502,11 @@
         <v>7.6500000000000005E-3</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E15" si="2">0.0002*ABS(C4)+0.00000005</f>
-        <v>5.1999999999999996E-8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <f t="shared" ref="E4:E14" si="2">0.0002*ABS(C4)+0.00005</f>
+        <v>5.0002E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-1.2</v>
       </c>
@@ -523,10 +523,10 @@
       </c>
       <c r="E5">
         <f t="shared" si="2"/>
-        <v>5.1999999999999996E-8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>5.0002E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-1.1000000000000001</v>
       </c>
@@ -543,10 +543,10 @@
       </c>
       <c r="E6">
         <f t="shared" si="2"/>
-        <v>5.1999999999999996E-8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>5.0002E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-1</v>
       </c>
@@ -563,10 +563,10 @@
       </c>
       <c r="E7">
         <f t="shared" si="2"/>
-        <v>5.1999999999999996E-8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>5.0002E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-0.9</v>
       </c>
@@ -583,10 +583,10 @@
       </c>
       <c r="E8">
         <f t="shared" si="2"/>
-        <v>5.1999999999999996E-8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>5.0002E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-0.8</v>
       </c>
@@ -603,10 +603,10 @@
       </c>
       <c r="E9">
         <f t="shared" si="2"/>
-        <v>5.1999999999999996E-8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>5.0002E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-0.7</v>
       </c>
@@ -623,10 +623,10 @@
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
-        <v>5.1999999999999996E-8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+        <v>5.0002E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-0.6</v>
       </c>
@@ -643,10 +643,10 @@
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
-        <v>5.1999999999999996E-8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+        <v>5.0002E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>-0.5</v>
       </c>
@@ -663,10 +663,10 @@
       </c>
       <c r="E12">
         <f t="shared" si="2"/>
-        <v>5.1999999999999996E-8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+        <v>5.0002E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>-0.4</v>
       </c>
@@ -683,10 +683,10 @@
       </c>
       <c r="E13">
         <f t="shared" si="2"/>
-        <v>5.1999999999999996E-8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+        <v>5.0002E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>-0.1</v>
       </c>
@@ -703,10 +703,10 @@
       </c>
       <c r="E14">
         <f t="shared" si="2"/>
-        <v>5.1999999999999996E-8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+        <v>5.0002E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -721,11 +721,11 @@
         <v>2.0200000000000003E-5</v>
       </c>
       <c r="E15">
-        <f t="shared" si="2"/>
-        <v>4.9999999999999998E-8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+        <f>0.002*ABS(C15)+0.00005</f>
+        <v>5.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.1</v>
       </c>
@@ -740,11 +740,11 @@
         <v>1.0009999999999999E-4</v>
       </c>
       <c r="E16">
-        <f>0.0002*ABS(C16)+0.00000005</f>
-        <v>2.5000000000000004E-7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+        <f t="shared" ref="E16:E18" si="3">0.002*ABS(C16)+0.00005</f>
+        <v>5.2000000000000004E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0.4</v>
       </c>
@@ -759,11 +759,11 @@
         <v>6.9990000000000004E-4</v>
       </c>
       <c r="E17">
-        <f>0.0002*ABS(C17)+0.00000005</f>
-        <v>1.8499999999999999E-6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+        <f t="shared" si="3"/>
+        <v>6.7999999999999999E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0.5</v>
       </c>
@@ -774,15 +774,15 @@
         <v>0.114</v>
       </c>
       <c r="D18">
-        <f t="shared" ref="D18:D27" si="3">0.0005*B18+0.0005</f>
+        <f t="shared" ref="D18:D27" si="4">0.0005*B18+0.0005</f>
         <v>7.5000000000000002E-4</v>
       </c>
       <c r="E18">
-        <f t="shared" ref="E18" si="4">0.0002*ABS(C18)+0.00000005</f>
-        <v>2.2850000000000003E-5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+        <f t="shared" si="3"/>
+        <v>2.7800000000000004E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0.6</v>
       </c>
@@ -793,15 +793,15 @@
         <v>0.95499999999999996</v>
       </c>
       <c r="D19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.9894999999999999E-4</v>
       </c>
       <c r="E19">
-        <f>0.0002*ABS(C19)+0.0000005</f>
-        <v>1.9150000000000002E-4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+        <f>0.002*ABS(C19)+0.0005</f>
+        <v>2.4099999999999998E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0.7</v>
       </c>
@@ -812,15 +812,15 @@
         <v>6.0629999999999997</v>
       </c>
       <c r="D20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.4314999999999998E-4</v>
       </c>
       <c r="E20">
-        <f>0.0002*ABS(C20)+0.000005</f>
-        <v>1.2176000000000001E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+        <f>0.002*ABS(C20)+0.005</f>
+        <v>1.7125999999999999E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0.8</v>
       </c>
@@ -831,15 +831,15 @@
         <v>23.974</v>
       </c>
       <c r="D21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.7399999999999999E-4</v>
       </c>
       <c r="E21">
-        <f t="shared" ref="E21:E22" si="5">0.0002*ABS(C21)+0.000005</f>
-        <v>4.7997999999999999E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+        <f>0.002*ABS(C21)+0.005</f>
+        <v>5.2948000000000002E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0.9</v>
       </c>
@@ -850,15 +850,15 @@
         <v>53.91</v>
       </c>
       <c r="D22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.9115000000000006E-4</v>
       </c>
       <c r="E22">
-        <f t="shared" si="5"/>
-        <v>1.0787E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+        <f>0.002*ABS(C22)+0.05</f>
+        <v>0.15782000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -869,15 +869,15 @@
         <v>90.53</v>
       </c>
       <c r="D23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.0115000000000008E-4</v>
       </c>
       <c r="E23">
-        <f>0.0002*ABS(C23)+0.00005</f>
-        <v>1.8156000000000002E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+        <f t="shared" ref="E23:E27" si="5">0.002*ABS(C23)+0.05</f>
+        <v>0.23105999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1.1000000000000001</v>
       </c>
@@ -888,15 +888,15 @@
         <v>129.54</v>
       </c>
       <c r="D24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.0795000000000003E-4</v>
       </c>
       <c r="E24">
-        <f t="shared" ref="E24:E27" si="6">0.0002*ABS(C24)+0.00005</f>
-        <v>2.5958000000000002E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+        <f t="shared" si="5"/>
+        <v>0.30907999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1.2</v>
       </c>
@@ -907,15 +907,15 @@
         <v>170.11</v>
       </c>
       <c r="D25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.1280000000000007E-4</v>
       </c>
       <c r="E25">
-        <f t="shared" si="6"/>
-        <v>3.4072000000000005E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+        <f t="shared" si="5"/>
+        <v>0.39022000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1.3</v>
       </c>
@@ -926,15 +926,15 @@
         <v>211.31</v>
       </c>
       <c r="D26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.1639999999999994E-4</v>
       </c>
       <c r="E26">
-        <f t="shared" si="6"/>
-        <v>4.2312000000000002E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+        <f t="shared" si="5"/>
+        <v>0.47261999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1.4</v>
       </c>
@@ -945,12 +945,12 @@
         <v>252.5</v>
       </c>
       <c r="D27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.1945000000000004E-4</v>
       </c>
       <c r="E27">
-        <f t="shared" si="6"/>
-        <v>5.0550000000000005E-2</v>
+        <f t="shared" si="5"/>
+        <v>0.55500000000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>